<commit_message>
Expert prices new db design
</commit_message>
<xml_diff>
--- a/templates/report/precios.xlsx
+++ b/templates/report/precios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Development\projects\ciber\cotown\back\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Development\projects\ciber\cotown\back\templates\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{261FE050-1BEB-4E5D-B407-A77EB1D88DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41B9EE8-1296-415E-B4BF-5028831F5D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Precios" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Precios!$A$2:$K$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Precios!$A$2:$M$3</definedName>
   </definedNames>
-  <calcPr calcId="0" iterate="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Año</t>
   </si>
@@ -98,6 +98,15 @@
   </si>
   <si>
     <t>.</t>
+  </si>
+  <si>
+    <t>Building.Code</t>
+  </si>
+  <si>
+    <t>Edificio</t>
+  </si>
+  <si>
+    <t>Building.Name</t>
   </si>
 </sst>
 </file>
@@ -615,111 +624,123 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24.85546875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="2" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="14" width="17.7109375" style="2" customWidth="1"/>
-    <col min="15" max="16384" width="24.85546875" style="2"/>
+    <col min="5" max="5" width="24.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="40.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16" width="17.7109375" style="2" customWidth="1"/>
+    <col min="17" max="16384" width="24.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6"/>
+      <c r="F1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="6"/>
+      <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4"/>
+      <c r="F2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="4"/>
+      <c r="H2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -727,10 +748,12 @@
       <c r="L3" s="9"/>
       <c r="M3" s="9"/>
       <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
     </row>
-    <row r="4" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="A2:K3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A2:M3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>